<commit_message>
CRM exports - Feat 8834 (#8891)
* fix too many requests

* WIP #8834

* movie type to static models

* WIP release media

* debug hasFilmography pipe

* column for the creation date of the organization

* fixed analytics export

* debug for user analytics export

* WIP blockframesadmin can export all contracts

* blockframesAdmin can export all offers

* updated releaseMedia list

* typo

* WIP

* cleaning

Co-authored-by: bruce <delorme.bruce.michel@gmail.com>
</commit_message>
<xml_diff>
--- a/assets/templates/import-titles-seller-template.xlsx
+++ b/assets/templates/import-titles-seller-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Documents\blockframes\assets\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincent/Dropbox/Mon Mac (MacBook Pro de Vincent)/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29339242-6079-4B2F-9347-3E2F68B4109C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39BE214-DF03-3345-8942-F8E216E2A018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="885" windowWidth="29040" windowHeight="15465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="28800" windowHeight="15460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Film metadata" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="547">
   <si>
     <t>Import Titles (Metadata)</t>
   </si>
@@ -2282,6 +2282,12 @@
   </si>
   <si>
     <t>EOF (French Speaking Films)</t>
+  </si>
+  <si>
+    <t>S-VOD</t>
+  </si>
+  <si>
+    <t>Festival</t>
   </si>
 </sst>
 </file>
@@ -2678,7 +2684,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="76">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2818,19 +2824,20 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2838,12 +2845,11 @@
     <xf numFmtId="49" fontId="8" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3071,49 +3077,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BT1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="14" topLeftCell="AK15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
       <selection pane="bottomRight" activeCell="AT6" sqref="AT6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" customWidth="1"/>
-    <col min="2" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="28.3984375" customWidth="1"/>
+    <col min="2" max="3" width="30.796875" customWidth="1"/>
+    <col min="4" max="4" width="34.796875" customWidth="1"/>
     <col min="5" max="7" width="39" customWidth="1"/>
-    <col min="8" max="8" width="35.7109375" customWidth="1"/>
-    <col min="9" max="9" width="26.85546875" customWidth="1"/>
-    <col min="10" max="10" width="58.28515625" customWidth="1"/>
-    <col min="11" max="11" width="33.42578125" customWidth="1"/>
-    <col min="12" max="12" width="30.7109375" customWidth="1"/>
-    <col min="13" max="14" width="25.7109375" customWidth="1"/>
+    <col min="8" max="8" width="35.796875" customWidth="1"/>
+    <col min="9" max="9" width="26.796875" customWidth="1"/>
+    <col min="10" max="10" width="58.19921875" customWidth="1"/>
+    <col min="11" max="11" width="33.3984375" customWidth="1"/>
+    <col min="12" max="12" width="30.796875" customWidth="1"/>
+    <col min="13" max="14" width="25.796875" customWidth="1"/>
     <col min="15" max="15" width="32" customWidth="1"/>
-    <col min="16" max="16" width="31.42578125" customWidth="1"/>
-    <col min="17" max="17" width="53.85546875" customWidth="1"/>
-    <col min="18" max="18" width="39.85546875" customWidth="1"/>
-    <col min="19" max="19" width="25.7109375" customWidth="1"/>
-    <col min="20" max="20" width="31.42578125" customWidth="1"/>
-    <col min="21" max="28" width="25.7109375" customWidth="1"/>
-    <col min="29" max="29" width="32.28515625" customWidth="1"/>
-    <col min="30" max="30" width="31.7109375" customWidth="1"/>
-    <col min="31" max="31" width="29.42578125" customWidth="1"/>
-    <col min="32" max="33" width="46.7109375" customWidth="1"/>
-    <col min="34" max="35" width="25.7109375" customWidth="1"/>
-    <col min="36" max="36" width="21.140625" customWidth="1"/>
-    <col min="37" max="37" width="25.7109375" customWidth="1"/>
-    <col min="38" max="38" width="20.42578125" customWidth="1"/>
-    <col min="39" max="39" width="23.42578125" customWidth="1"/>
-    <col min="40" max="49" width="16.5703125" customWidth="1"/>
-    <col min="50" max="50" width="21.140625" customWidth="1"/>
-    <col min="51" max="63" width="16.5703125" customWidth="1"/>
-    <col min="64" max="64" width="46.7109375" customWidth="1"/>
-    <col min="65" max="72" width="16.5703125" customWidth="1"/>
+    <col min="16" max="16" width="31.3984375" customWidth="1"/>
+    <col min="17" max="17" width="53.796875" customWidth="1"/>
+    <col min="18" max="18" width="39.796875" customWidth="1"/>
+    <col min="19" max="19" width="25.796875" customWidth="1"/>
+    <col min="20" max="20" width="31.3984375" customWidth="1"/>
+    <col min="21" max="28" width="25.796875" customWidth="1"/>
+    <col min="29" max="29" width="32.19921875" customWidth="1"/>
+    <col min="30" max="30" width="31.796875" customWidth="1"/>
+    <col min="31" max="31" width="29.3984375" customWidth="1"/>
+    <col min="32" max="33" width="46.796875" customWidth="1"/>
+    <col min="34" max="35" width="25.796875" customWidth="1"/>
+    <col min="36" max="36" width="21.19921875" customWidth="1"/>
+    <col min="37" max="37" width="25.796875" customWidth="1"/>
+    <col min="38" max="38" width="20.3984375" customWidth="1"/>
+    <col min="39" max="39" width="23.3984375" customWidth="1"/>
+    <col min="40" max="49" width="16.59765625" customWidth="1"/>
+    <col min="50" max="50" width="21.19921875" customWidth="1"/>
+    <col min="51" max="63" width="16.59765625" customWidth="1"/>
+    <col min="64" max="64" width="46.796875" customWidth="1"/>
+    <col min="65" max="72" width="16.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:72" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:72" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
@@ -3136,7 +3142,7 @@
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
     </row>
-    <row r="2" spans="1:72" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:72" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -3161,7 +3167,7 @@
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
     </row>
-    <row r="3" spans="1:72" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:72" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -3184,7 +3190,7 @@
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
     </row>
-    <row r="4" spans="1:72" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:72" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>1</v>
       </c>
@@ -3209,15 +3215,15 @@
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
     </row>
-    <row r="5" spans="1:72" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="70" t="s">
+    <row r="5" spans="1:72" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
@@ -3234,15 +3240,15 @@
       <c r="T5" s="3"/>
       <c r="U5" s="3"/>
     </row>
-    <row r="6" spans="1:72" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="72" t="s">
+    <row r="6" spans="1:72" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="71"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
@@ -3259,7 +3265,7 @@
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
     </row>
-    <row r="7" spans="1:72" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:72" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -3282,7 +3288,7 @@
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
     </row>
-    <row r="8" spans="1:72" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:72" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
       <c r="B8" s="15"/>
       <c r="C8" s="9"/>
@@ -3305,7 +3311,7 @@
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
     </row>
-    <row r="9" spans="1:72" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:72" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17"/>
       <c r="B9" s="18"/>
       <c r="C9" s="18"/>
@@ -3328,7 +3334,7 @@
       <c r="T9" s="3"/>
       <c r="U9" s="3"/>
     </row>
-    <row r="10" spans="1:72" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:72" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="20"/>
       <c r="B10" s="20"/>
       <c r="C10" s="21"/>
@@ -3402,7 +3408,7 @@
       <c r="BS10" s="24"/>
       <c r="BT10" s="24"/>
     </row>
-    <row r="11" spans="1:72" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:72" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="20"/>
       <c r="B11" s="20"/>
       <c r="C11" s="21"/>
@@ -3476,7 +3482,7 @@
       <c r="BS11" s="24"/>
       <c r="BT11" s="24"/>
     </row>
-    <row r="12" spans="1:72" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:72" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="20"/>
       <c r="B12" s="20"/>
       <c r="C12" s="21"/>
@@ -3550,7 +3556,7 @@
       <c r="BS12" s="24"/>
       <c r="BT12" s="24"/>
     </row>
-    <row r="13" spans="1:72" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:72" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="20"/>
       <c r="B13" s="20"/>
       <c r="C13" s="21"/>
@@ -3819,15 +3825,15 @@
       </c>
     </row>
     <row r="15" spans="1:72" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="67"/>
-      <c r="B15" s="67"/>
-      <c r="C15" s="67"/>
-      <c r="D15" s="67"/>
-      <c r="E15" s="67"/>
-      <c r="F15" s="67"/>
-      <c r="G15" s="67"/>
-      <c r="H15" s="68"/>
-      <c r="I15" s="67"/>
+      <c r="A15" s="65"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="69"/>
+      <c r="I15" s="65"/>
       <c r="J15" s="33"/>
       <c r="K15" s="33"/>
       <c r="L15" s="33"/>
@@ -3841,8 +3847,8 @@
       <c r="T15" s="33"/>
       <c r="U15" s="33"/>
       <c r="V15" s="33"/>
-      <c r="W15" s="69"/>
-      <c r="X15" s="67"/>
+      <c r="W15" s="70"/>
+      <c r="X15" s="65"/>
       <c r="Y15" s="33"/>
       <c r="Z15" s="33"/>
       <c r="AA15" s="33"/>
@@ -3850,9 +3856,9 @@
       <c r="AC15" s="34"/>
       <c r="AD15" s="33"/>
       <c r="AE15" s="33"/>
-      <c r="AF15" s="67"/>
-      <c r="AG15" s="67"/>
-      <c r="AH15" s="67"/>
+      <c r="AF15" s="65"/>
+      <c r="AG15" s="65"/>
+      <c r="AH15" s="65"/>
       <c r="AI15" s="33"/>
       <c r="AJ15" s="33"/>
       <c r="AK15" s="33"/>
@@ -3860,7 +3866,7 @@
       <c r="AM15" s="33"/>
       <c r="AN15" s="33"/>
       <c r="AO15" s="33"/>
-      <c r="AP15" s="67"/>
+      <c r="AP15" s="65"/>
       <c r="AQ15" s="33"/>
       <c r="AR15" s="33"/>
       <c r="AS15" s="33"/>
@@ -3873,16 +3879,16 @@
       <c r="AZ15" s="33"/>
       <c r="BA15" s="33"/>
       <c r="BB15" s="33"/>
-      <c r="BC15" s="67"/>
-      <c r="BD15" s="67"/>
-      <c r="BE15" s="67"/>
-      <c r="BF15" s="67"/>
-      <c r="BG15" s="67"/>
+      <c r="BC15" s="65"/>
+      <c r="BD15" s="65"/>
+      <c r="BE15" s="65"/>
+      <c r="BF15" s="65"/>
+      <c r="BG15" s="65"/>
       <c r="BH15" s="33"/>
       <c r="BI15" s="33"/>
       <c r="BJ15" s="33"/>
       <c r="BK15" s="33"/>
-      <c r="BL15" s="67"/>
+      <c r="BL15" s="65"/>
       <c r="BM15" s="35"/>
       <c r="BN15" s="35"/>
       <c r="BO15" s="35"/>
@@ -4559,15 +4565,15 @@
       <c r="BT24" s="14"/>
     </row>
     <row r="25" spans="1:72" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="65"/>
-      <c r="B25" s="65"/>
-      <c r="C25" s="65"/>
-      <c r="D25" s="65"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="65"/>
-      <c r="G25" s="65"/>
-      <c r="H25" s="62"/>
-      <c r="I25" s="65"/>
+      <c r="A25" s="62"/>
+      <c r="B25" s="62"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="62"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="71"/>
+      <c r="I25" s="62"/>
       <c r="J25" s="39"/>
       <c r="K25" s="39"/>
       <c r="L25" s="39"/>
@@ -4581,8 +4587,8 @@
       <c r="T25" s="39"/>
       <c r="U25" s="39"/>
       <c r="V25" s="39"/>
-      <c r="W25" s="66"/>
-      <c r="X25" s="65"/>
+      <c r="W25" s="72"/>
+      <c r="X25" s="62"/>
       <c r="Y25" s="39"/>
       <c r="Z25" s="39"/>
       <c r="AA25" s="39"/>
@@ -4590,9 +4596,9 @@
       <c r="AC25" s="40"/>
       <c r="AD25" s="39"/>
       <c r="AE25" s="39"/>
-      <c r="AF25" s="65"/>
-      <c r="AG25" s="65"/>
-      <c r="AH25" s="65"/>
+      <c r="AF25" s="62"/>
+      <c r="AG25" s="62"/>
+      <c r="AH25" s="62"/>
       <c r="AI25" s="39"/>
       <c r="AJ25" s="39"/>
       <c r="AK25" s="39"/>
@@ -4600,7 +4606,7 @@
       <c r="AM25" s="39"/>
       <c r="AN25" s="39"/>
       <c r="AO25" s="39"/>
-      <c r="AP25" s="65"/>
+      <c r="AP25" s="62"/>
       <c r="AQ25" s="39"/>
       <c r="AR25" s="39"/>
       <c r="AS25" s="39"/>
@@ -4613,16 +4619,16 @@
       <c r="AZ25" s="39"/>
       <c r="BA25" s="39"/>
       <c r="BB25" s="39"/>
-      <c r="BC25" s="65"/>
-      <c r="BD25" s="65"/>
-      <c r="BE25" s="65"/>
-      <c r="BF25" s="65"/>
-      <c r="BG25" s="65"/>
+      <c r="BC25" s="62"/>
+      <c r="BD25" s="62"/>
+      <c r="BE25" s="62"/>
+      <c r="BF25" s="62"/>
+      <c r="BG25" s="62"/>
       <c r="BH25" s="39"/>
       <c r="BI25" s="39"/>
       <c r="BJ25" s="39"/>
       <c r="BK25" s="39"/>
-      <c r="BL25" s="65"/>
+      <c r="BL25" s="62"/>
       <c r="BM25" s="42"/>
       <c r="BN25" s="42"/>
       <c r="BO25" s="42"/>
@@ -5303,8 +5309,8 @@
       <c r="B35" s="73"/>
       <c r="C35" s="73"/>
       <c r="D35" s="73"/>
-      <c r="E35" s="67"/>
-      <c r="F35" s="67"/>
+      <c r="E35" s="65"/>
+      <c r="F35" s="65"/>
       <c r="G35" s="73"/>
       <c r="H35" s="74"/>
       <c r="I35" s="73"/>
@@ -6039,15 +6045,15 @@
       <c r="BT44" s="14"/>
     </row>
     <row r="45" spans="1:72" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="65"/>
-      <c r="B45" s="65"/>
-      <c r="C45" s="65"/>
-      <c r="D45" s="65"/>
-      <c r="E45" s="65"/>
-      <c r="F45" s="65"/>
-      <c r="G45" s="65"/>
-      <c r="H45" s="62"/>
-      <c r="I45" s="65"/>
+      <c r="A45" s="62"/>
+      <c r="B45" s="62"/>
+      <c r="C45" s="62"/>
+      <c r="D45" s="62"/>
+      <c r="E45" s="62"/>
+      <c r="F45" s="62"/>
+      <c r="G45" s="62"/>
+      <c r="H45" s="71"/>
+      <c r="I45" s="62"/>
       <c r="J45" s="39"/>
       <c r="K45" s="39"/>
       <c r="L45" s="39"/>
@@ -6061,8 +6067,8 @@
       <c r="T45" s="39"/>
       <c r="U45" s="39"/>
       <c r="V45" s="39"/>
-      <c r="W45" s="66"/>
-      <c r="X45" s="65"/>
+      <c r="W45" s="72"/>
+      <c r="X45" s="62"/>
       <c r="Y45" s="39"/>
       <c r="Z45" s="39"/>
       <c r="AA45" s="39"/>
@@ -6070,9 +6076,9 @@
       <c r="AC45" s="40"/>
       <c r="AD45" s="39"/>
       <c r="AE45" s="39"/>
-      <c r="AF45" s="65"/>
-      <c r="AG45" s="65"/>
-      <c r="AH45" s="65"/>
+      <c r="AF45" s="62"/>
+      <c r="AG45" s="62"/>
+      <c r="AH45" s="62"/>
       <c r="AI45" s="39"/>
       <c r="AJ45" s="39"/>
       <c r="AK45" s="39"/>
@@ -6080,7 +6086,7 @@
       <c r="AM45" s="39"/>
       <c r="AN45" s="39"/>
       <c r="AO45" s="39"/>
-      <c r="AP45" s="65"/>
+      <c r="AP45" s="62"/>
       <c r="AQ45" s="39"/>
       <c r="AR45" s="39"/>
       <c r="AS45" s="39"/>
@@ -6093,16 +6099,16 @@
       <c r="AZ45" s="39"/>
       <c r="BA45" s="39"/>
       <c r="BB45" s="39"/>
-      <c r="BC45" s="65"/>
-      <c r="BD45" s="65"/>
-      <c r="BE45" s="65"/>
-      <c r="BF45" s="65"/>
-      <c r="BG45" s="65"/>
+      <c r="BC45" s="62"/>
+      <c r="BD45" s="62"/>
+      <c r="BE45" s="62"/>
+      <c r="BF45" s="62"/>
+      <c r="BG45" s="62"/>
       <c r="BH45" s="39"/>
       <c r="BI45" s="39"/>
       <c r="BJ45" s="39"/>
       <c r="BK45" s="39"/>
-      <c r="BL45" s="65"/>
+      <c r="BL45" s="62"/>
       <c r="BM45" s="42"/>
       <c r="BN45" s="42"/>
       <c r="BO45" s="42"/>
@@ -6783,8 +6789,8 @@
       <c r="B55" s="73"/>
       <c r="C55" s="73"/>
       <c r="D55" s="73"/>
-      <c r="E55" s="67"/>
-      <c r="F55" s="67"/>
+      <c r="E55" s="65"/>
+      <c r="F55" s="65"/>
       <c r="G55" s="73"/>
       <c r="H55" s="74"/>
       <c r="I55" s="73"/>
@@ -7519,15 +7525,15 @@
       <c r="BT64" s="14"/>
     </row>
     <row r="65" spans="1:72" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="65"/>
-      <c r="B65" s="65"/>
-      <c r="C65" s="65"/>
-      <c r="D65" s="65"/>
-      <c r="E65" s="65"/>
-      <c r="F65" s="65"/>
-      <c r="G65" s="65"/>
-      <c r="H65" s="62"/>
-      <c r="I65" s="65"/>
+      <c r="A65" s="62"/>
+      <c r="B65" s="62"/>
+      <c r="C65" s="62"/>
+      <c r="D65" s="62"/>
+      <c r="E65" s="62"/>
+      <c r="F65" s="62"/>
+      <c r="G65" s="62"/>
+      <c r="H65" s="71"/>
+      <c r="I65" s="62"/>
       <c r="J65" s="39"/>
       <c r="K65" s="39"/>
       <c r="L65" s="39"/>
@@ -7541,8 +7547,8 @@
       <c r="T65" s="39"/>
       <c r="U65" s="39"/>
       <c r="V65" s="39"/>
-      <c r="W65" s="66"/>
-      <c r="X65" s="65"/>
+      <c r="W65" s="72"/>
+      <c r="X65" s="62"/>
       <c r="Y65" s="39"/>
       <c r="Z65" s="39"/>
       <c r="AA65" s="39"/>
@@ -7550,9 +7556,9 @@
       <c r="AC65" s="40"/>
       <c r="AD65" s="39"/>
       <c r="AE65" s="39"/>
-      <c r="AF65" s="65"/>
-      <c r="AG65" s="65"/>
-      <c r="AH65" s="65"/>
+      <c r="AF65" s="62"/>
+      <c r="AG65" s="62"/>
+      <c r="AH65" s="62"/>
       <c r="AI65" s="39"/>
       <c r="AJ65" s="39"/>
       <c r="AK65" s="39"/>
@@ -7560,7 +7566,7 @@
       <c r="AM65" s="39"/>
       <c r="AN65" s="39"/>
       <c r="AO65" s="39"/>
-      <c r="AP65" s="65"/>
+      <c r="AP65" s="62"/>
       <c r="AQ65" s="39"/>
       <c r="AR65" s="39"/>
       <c r="AS65" s="39"/>
@@ -7573,16 +7579,16 @@
       <c r="AZ65" s="39"/>
       <c r="BA65" s="39"/>
       <c r="BB65" s="39"/>
-      <c r="BC65" s="65"/>
-      <c r="BD65" s="65"/>
-      <c r="BE65" s="65"/>
-      <c r="BF65" s="65"/>
-      <c r="BG65" s="65"/>
+      <c r="BC65" s="62"/>
+      <c r="BD65" s="62"/>
+      <c r="BE65" s="62"/>
+      <c r="BF65" s="62"/>
+      <c r="BG65" s="62"/>
       <c r="BH65" s="39"/>
       <c r="BI65" s="39"/>
       <c r="BJ65" s="39"/>
       <c r="BK65" s="39"/>
-      <c r="BL65" s="65"/>
+      <c r="BL65" s="62"/>
       <c r="BM65" s="42"/>
       <c r="BN65" s="42"/>
       <c r="BO65" s="42"/>
@@ -8263,8 +8269,8 @@
       <c r="B75" s="73"/>
       <c r="C75" s="73"/>
       <c r="D75" s="73"/>
-      <c r="E75" s="67"/>
-      <c r="F75" s="67"/>
+      <c r="E75" s="65"/>
+      <c r="F75" s="65"/>
       <c r="G75" s="73"/>
       <c r="H75" s="74"/>
       <c r="I75" s="73"/>
@@ -8999,15 +9005,15 @@
       <c r="BT84" s="14"/>
     </row>
     <row r="85" spans="1:72" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="65"/>
-      <c r="B85" s="65"/>
-      <c r="C85" s="65"/>
-      <c r="D85" s="65"/>
-      <c r="E85" s="65"/>
-      <c r="F85" s="65"/>
-      <c r="G85" s="65"/>
-      <c r="H85" s="62"/>
-      <c r="I85" s="65"/>
+      <c r="A85" s="62"/>
+      <c r="B85" s="62"/>
+      <c r="C85" s="62"/>
+      <c r="D85" s="62"/>
+      <c r="E85" s="62"/>
+      <c r="F85" s="62"/>
+      <c r="G85" s="62"/>
+      <c r="H85" s="71"/>
+      <c r="I85" s="62"/>
       <c r="J85" s="39"/>
       <c r="K85" s="39"/>
       <c r="L85" s="39"/>
@@ -9021,8 +9027,8 @@
       <c r="T85" s="39"/>
       <c r="U85" s="39"/>
       <c r="V85" s="39"/>
-      <c r="W85" s="66"/>
-      <c r="X85" s="65"/>
+      <c r="W85" s="72"/>
+      <c r="X85" s="62"/>
       <c r="Y85" s="39"/>
       <c r="Z85" s="39"/>
       <c r="AA85" s="39"/>
@@ -9030,9 +9036,9 @@
       <c r="AC85" s="40"/>
       <c r="AD85" s="39"/>
       <c r="AE85" s="39"/>
-      <c r="AF85" s="65"/>
-      <c r="AG85" s="65"/>
-      <c r="AH85" s="65"/>
+      <c r="AF85" s="62"/>
+      <c r="AG85" s="62"/>
+      <c r="AH85" s="62"/>
       <c r="AI85" s="39"/>
       <c r="AJ85" s="39"/>
       <c r="AK85" s="39"/>
@@ -9040,7 +9046,7 @@
       <c r="AM85" s="39"/>
       <c r="AN85" s="39"/>
       <c r="AO85" s="39"/>
-      <c r="AP85" s="65"/>
+      <c r="AP85" s="62"/>
       <c r="AQ85" s="39"/>
       <c r="AR85" s="39"/>
       <c r="AS85" s="39"/>
@@ -9053,16 +9059,16 @@
       <c r="AZ85" s="39"/>
       <c r="BA85" s="39"/>
       <c r="BB85" s="39"/>
-      <c r="BC85" s="65"/>
-      <c r="BD85" s="65"/>
-      <c r="BE85" s="65"/>
-      <c r="BF85" s="65"/>
-      <c r="BG85" s="65"/>
+      <c r="BC85" s="62"/>
+      <c r="BD85" s="62"/>
+      <c r="BE85" s="62"/>
+      <c r="BF85" s="62"/>
+      <c r="BG85" s="62"/>
       <c r="BH85" s="39"/>
       <c r="BI85" s="39"/>
       <c r="BJ85" s="39"/>
       <c r="BK85" s="39"/>
-      <c r="BL85" s="65"/>
+      <c r="BL85" s="62"/>
       <c r="BM85" s="42"/>
       <c r="BN85" s="42"/>
       <c r="BO85" s="42"/>
@@ -11397,6 +11403,13 @@
     <mergeCell ref="G85:G94"/>
     <mergeCell ref="H85:H94"/>
     <mergeCell ref="I85:I94"/>
+    <mergeCell ref="C75:C84"/>
+    <mergeCell ref="D75:D84"/>
+    <mergeCell ref="E75:E84"/>
+    <mergeCell ref="F75:F84"/>
+    <mergeCell ref="G75:G84"/>
+    <mergeCell ref="AP75:AP84"/>
+    <mergeCell ref="BC75:BC84"/>
     <mergeCell ref="W85:W94"/>
     <mergeCell ref="X85:X94"/>
     <mergeCell ref="AF85:AF94"/>
@@ -11408,15 +11421,6 @@
     <mergeCell ref="AF75:AF84"/>
     <mergeCell ref="AG75:AG84"/>
     <mergeCell ref="AH75:AH84"/>
-    <mergeCell ref="A75:A84"/>
-    <mergeCell ref="B75:B84"/>
-    <mergeCell ref="C75:C84"/>
-    <mergeCell ref="D75:D84"/>
-    <mergeCell ref="E75:E84"/>
-    <mergeCell ref="F75:F84"/>
-    <mergeCell ref="G75:G84"/>
-    <mergeCell ref="AP75:AP84"/>
-    <mergeCell ref="BC75:BC84"/>
     <mergeCell ref="BD75:BD84"/>
     <mergeCell ref="BE75:BE84"/>
     <mergeCell ref="BF75:BF84"/>
@@ -11439,6 +11443,8 @@
     <mergeCell ref="H75:H84"/>
     <mergeCell ref="I75:I84"/>
     <mergeCell ref="W75:W84"/>
+    <mergeCell ref="A75:A84"/>
+    <mergeCell ref="B75:B84"/>
     <mergeCell ref="BF65:BF74"/>
     <mergeCell ref="BG65:BG74"/>
     <mergeCell ref="BL65:BL74"/>
@@ -11481,8 +11487,6 @@
     <mergeCell ref="AF55:AF64"/>
     <mergeCell ref="AG55:AG64"/>
     <mergeCell ref="AH55:AH64"/>
-    <mergeCell ref="BD45:BD54"/>
-    <mergeCell ref="BE45:BE54"/>
     <mergeCell ref="BF45:BF54"/>
     <mergeCell ref="BG45:BG54"/>
     <mergeCell ref="BL45:BL54"/>
@@ -11502,6 +11506,22 @@
     <mergeCell ref="AH45:AH54"/>
     <mergeCell ref="AP45:AP54"/>
     <mergeCell ref="BC45:BC54"/>
+    <mergeCell ref="A35:A44"/>
+    <mergeCell ref="B35:B44"/>
+    <mergeCell ref="C35:C44"/>
+    <mergeCell ref="D35:D44"/>
+    <mergeCell ref="E35:E44"/>
+    <mergeCell ref="F35:F44"/>
+    <mergeCell ref="G35:G44"/>
+    <mergeCell ref="BD45:BD54"/>
+    <mergeCell ref="BE45:BE54"/>
+    <mergeCell ref="AP35:AP44"/>
+    <mergeCell ref="BC35:BC44"/>
+    <mergeCell ref="BD35:BD44"/>
+    <mergeCell ref="BE35:BE44"/>
+    <mergeCell ref="BF35:BF44"/>
+    <mergeCell ref="BG35:BG44"/>
+    <mergeCell ref="BL35:BL44"/>
     <mergeCell ref="H35:H44"/>
     <mergeCell ref="I35:I44"/>
     <mergeCell ref="W35:W44"/>
@@ -11509,25 +11529,6 @@
     <mergeCell ref="AF35:AF44"/>
     <mergeCell ref="AG35:AG44"/>
     <mergeCell ref="AH35:AH44"/>
-    <mergeCell ref="A35:A44"/>
-    <mergeCell ref="B35:B44"/>
-    <mergeCell ref="C35:C44"/>
-    <mergeCell ref="D35:D44"/>
-    <mergeCell ref="E35:E44"/>
-    <mergeCell ref="F35:F44"/>
-    <mergeCell ref="G35:G44"/>
-    <mergeCell ref="BD25:BD34"/>
-    <mergeCell ref="BE25:BE34"/>
-    <mergeCell ref="BF25:BF34"/>
-    <mergeCell ref="BG25:BG34"/>
-    <mergeCell ref="BL25:BL34"/>
-    <mergeCell ref="AP35:AP44"/>
-    <mergeCell ref="BC35:BC44"/>
-    <mergeCell ref="BD35:BD44"/>
-    <mergeCell ref="BE35:BE44"/>
-    <mergeCell ref="BF35:BF44"/>
-    <mergeCell ref="BG35:BG44"/>
-    <mergeCell ref="BL35:BL44"/>
     <mergeCell ref="A5:F5"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="A15:A24"/>
@@ -11544,15 +11545,6 @@
     <mergeCell ref="W15:W24"/>
     <mergeCell ref="X15:X24"/>
     <mergeCell ref="AF15:AF24"/>
-    <mergeCell ref="BG15:BG24"/>
-    <mergeCell ref="BL15:BL24"/>
-    <mergeCell ref="AG15:AG24"/>
-    <mergeCell ref="AH15:AH24"/>
-    <mergeCell ref="AP15:AP24"/>
-    <mergeCell ref="BC15:BC24"/>
-    <mergeCell ref="BD15:BD24"/>
-    <mergeCell ref="BE15:BE24"/>
-    <mergeCell ref="BF15:BF24"/>
     <mergeCell ref="H25:H34"/>
     <mergeCell ref="I25:I34"/>
     <mergeCell ref="W25:W34"/>
@@ -11567,6 +11559,20 @@
     <mergeCell ref="E25:E34"/>
     <mergeCell ref="F25:F34"/>
     <mergeCell ref="G25:G34"/>
+    <mergeCell ref="BG15:BG24"/>
+    <mergeCell ref="BL15:BL24"/>
+    <mergeCell ref="AG15:AG24"/>
+    <mergeCell ref="AH15:AH24"/>
+    <mergeCell ref="AP15:AP24"/>
+    <mergeCell ref="BC15:BC24"/>
+    <mergeCell ref="BD15:BD24"/>
+    <mergeCell ref="BE15:BE24"/>
+    <mergeCell ref="BF15:BF24"/>
+    <mergeCell ref="BD25:BD34"/>
+    <mergeCell ref="BE25:BE34"/>
+    <mergeCell ref="BF25:BF34"/>
+    <mergeCell ref="BG25:BG34"/>
+    <mergeCell ref="BL25:BL34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -11721,20 +11727,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23.796875" customWidth="1"/>
+    <col min="2" max="2" width="30.796875" customWidth="1"/>
+    <col min="3" max="3" width="28.19921875" customWidth="1"/>
     <col min="4" max="4" width="54" customWidth="1"/>
-    <col min="5" max="18" width="23.85546875" customWidth="1"/>
-    <col min="19" max="19" width="37.5703125" customWidth="1"/>
-    <col min="20" max="25" width="23.85546875" customWidth="1"/>
-    <col min="26" max="26" width="16.5703125" customWidth="1"/>
+    <col min="5" max="18" width="23.796875" customWidth="1"/>
+    <col min="19" max="19" width="37.59765625" customWidth="1"/>
+    <col min="20" max="25" width="23.796875" customWidth="1"/>
+    <col min="26" max="26" width="16.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -12102,7 +12108,9 @@
       <c r="B6" s="50" t="s">
         <v>170</v>
       </c>
-      <c r="C6" s="53"/>
+      <c r="C6" s="53" t="s">
+        <v>545</v>
+      </c>
       <c r="D6" s="50" t="s">
         <v>171</v>
       </c>
@@ -12153,7 +12161,9 @@
       <c r="B7" s="50" t="s">
         <v>181</v>
       </c>
-      <c r="C7" s="55"/>
+      <c r="C7" s="55" t="s">
+        <v>546</v>
+      </c>
       <c r="D7" s="50" t="s">
         <v>182</v>
       </c>
@@ -12195,7 +12205,7 @@
       <c r="X7" s="50"/>
       <c r="Y7" s="50"/>
     </row>
-    <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="50" t="s">
         <v>191</v>
       </c>
@@ -12242,7 +12252,7 @@
       <c r="X8" s="50"/>
       <c r="Y8" s="50"/>
     </row>
-    <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="50" t="s">
         <v>201</v>
       </c>
@@ -12285,7 +12295,7 @@
       <c r="X9" s="50"/>
       <c r="Y9" s="50"/>
     </row>
-    <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="50" t="s">
         <v>209</v>
       </c>
@@ -12326,7 +12336,7 @@
       <c r="X10" s="50"/>
       <c r="Y10" s="50"/>
     </row>
-    <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="50" t="s">
         <v>216</v>
       </c>
@@ -12365,7 +12375,7 @@
       <c r="X11" s="50"/>
       <c r="Y11" s="50"/>
     </row>
-    <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="50" t="s">
         <v>222</v>
       </c>
@@ -12404,7 +12414,7 @@
       <c r="X12" s="50"/>
       <c r="Y12" s="50"/>
     </row>
-    <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="50" t="s">
         <v>228</v>
       </c>
@@ -12443,7 +12453,7 @@
       <c r="X13" s="50"/>
       <c r="Y13" s="50"/>
     </row>
-    <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="50" t="s">
         <v>234</v>
       </c>
@@ -12480,7 +12490,7 @@
       <c r="X14" s="50"/>
       <c r="Y14" s="50"/>
     </row>
-    <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="50" t="s">
         <v>239</v>
       </c>
@@ -12515,7 +12525,7 @@
       <c r="X15" s="50"/>
       <c r="Y15" s="50"/>
     </row>
-    <row r="16" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="50" t="s">
         <v>243</v>
       </c>
@@ -12548,7 +12558,7 @@
       <c r="X16" s="50"/>
       <c r="Y16" s="50"/>
     </row>
-    <row r="17" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="50" t="s">
         <v>246</v>
       </c>
@@ -12581,7 +12591,7 @@
       <c r="X17" s="50"/>
       <c r="Y17" s="50"/>
     </row>
-    <row r="18" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="50" t="s">
         <v>249</v>
       </c>
@@ -12614,7 +12624,7 @@
       <c r="X18" s="50"/>
       <c r="Y18" s="50"/>
     </row>
-    <row r="19" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="50"/>
       <c r="B19" s="50"/>
       <c r="C19" s="53"/>
@@ -12645,7 +12655,7 @@
       <c r="X19" s="50"/>
       <c r="Y19" s="50"/>
     </row>
-    <row r="20" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="50"/>
       <c r="B20" s="50"/>
       <c r="C20" s="53"/>
@@ -12676,7 +12686,7 @@
       <c r="X20" s="50"/>
       <c r="Y20" s="50"/>
     </row>
-    <row r="21" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="50"/>
       <c r="B21" s="50"/>
       <c r="C21" s="53"/>
@@ -12707,7 +12717,7 @@
       <c r="X21" s="50"/>
       <c r="Y21" s="50"/>
     </row>
-    <row r="22" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="50"/>
       <c r="B22" s="50"/>
       <c r="C22" s="53"/>

</xml_diff>